<commit_message>
Update Design and Plan documents
</commit_message>
<xml_diff>
--- a/Project Plan/Plan Tables(risk filled out).xlsx
+++ b/Project Plan/Plan Tables(risk filled out).xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\barch_n8c1eh8\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jstitch\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9BA8BAF5-963E-4E32-B2EE-F4E833182EC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{220C5A5E-0385-4A0C-BFB1-E6B28DF7B5E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{F187870B-6DCA-47F1-99EA-BBA81ED883E2}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F187870B-6DCA-47F1-99EA-BBA81ED883E2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
   <si>
     <t>Risk</t>
   </si>
@@ -185,6 +185,12 @@
   </si>
   <si>
     <t>Test board rendering early. Print row/column labels, ensure loop indices match the visual grid, and validate that display formatting remains consistent after each move.</t>
+  </si>
+  <si>
+    <t>Jayden Brooks</t>
+  </si>
+  <si>
+    <t>Complete</t>
   </si>
 </sst>
 </file>
@@ -239,7 +245,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -257,6 +263,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
   </cellXfs>
@@ -595,16 +604,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A7042B5-177A-44F3-BC0C-86CAFAAA9A50}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="30.6640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="30.7109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="30.6640625" style="4"/>
+    <col min="1" max="16384" width="30.7109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -618,7 +627,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -632,7 +641,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="121.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -646,7 +655,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -660,7 +669,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -674,7 +683,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="99" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
@@ -688,7 +697,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
@@ -705,57 +714,81 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="7">
+        <v>45991</v>
+      </c>
+      <c r="D10" s="7">
+        <v>46011</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="7">
+        <v>45991</v>
+      </c>
+      <c r="D11" s="7">
+        <v>46011</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>24</v>
       </c>

</xml_diff>